<commit_message>
Added the color coding to the excel layout for the adjacecny list unit tests
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddierogers/Documents/Mines Spring 2017/CSCI306/ClueGameMRFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22785" windowHeight="10170"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26320" windowHeight="12260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="32">
   <si>
     <t>B</t>
   </si>
@@ -99,12 +102,33 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Number of doors: 19</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in BoardInitTests)</t>
+  </si>
+  <si>
+    <t>Orange: adjecency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adjecency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room enterance</t>
+  </si>
+  <si>
+    <t>Pink: walkway scenarios</t>
+  </si>
+  <si>
+    <t>light blue: test targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +169,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA89E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,18 +218,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA89E1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -444,16 +515,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -462,7 +533,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -477,7 +548,7 @@
       <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -498,7 +569,7 @@
       <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="10" t="s">
         <v>24</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -522,14 +593,14 @@
       <c r="W1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="Y1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +622,7 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -606,14 +677,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -664,7 +735,7 @@
       <c r="S3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="T3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U3" s="2" t="s">
@@ -683,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +794,7 @@
       <c r="M4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -760,7 +831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +975,7 @@
       <c r="V6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="X6" s="2" t="s">
@@ -914,8 +985,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -954,7 +1025,7 @@
       <c r="M7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O7" s="4" t="s">
@@ -991,7 +1062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1108,7 @@
       <c r="O8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="Q8" s="2" t="s">
@@ -1068,7 +1139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1145,7 +1216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1283,7 @@
       <c r="V10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="X10" s="2" t="s">
@@ -1222,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1312,7 @@
       <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1289,7 +1360,7 @@
       <c r="V11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="X11" s="2" t="s">
@@ -1299,7 +1370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1425,7 @@
       <c r="R12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="10" t="s">
         <v>24</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -1376,7 +1447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1425,7 +1496,7 @@
       <c r="P13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -1453,7 +1524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1484,7 +1555,7 @@
       <c r="J14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="8" t="s">
         <v>24</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -1530,7 +1601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1540,7 +1611,7 @@
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1549,7 +1620,7 @@
       <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1607,7 +1678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1617,7 +1688,7 @@
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1665,13 +1736,13 @@
       <c r="S16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="T16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V16" s="4" t="s">
+      <c r="V16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="W16" s="1" t="s">
@@ -1684,7 +1755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1761,7 +1832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1780,7 +1851,7 @@
       <c r="F18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -1810,7 +1881,7 @@
       <c r="P18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -1838,11 +1909,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1851,7 +1922,7 @@
       <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -1875,7 +1946,7 @@
       <c r="L19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="9" t="s">
         <v>23</v>
       </c>
       <c r="N19" s="2" t="s">
@@ -1896,7 +1967,7 @@
       <c r="S19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="T19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U19" s="4" t="s">
@@ -1915,7 +1986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1992,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -2079,7 +2150,7 @@
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -2112,7 +2183,7 @@
       <c r="N22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -2146,7 +2217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2218,6 +2289,41 @@
       </c>
       <c r="X23">
         <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote the unit tests for the target calculations and updated the excel sheet with tested cells highlighted
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="36">
   <si>
     <t>B</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Number of doors: 19</t>
   </si>
   <si>
-    <t>White: door direction tests (in BoardInitTests)</t>
-  </si>
-  <si>
     <t>Orange: adjecency list tests, inside room</t>
   </si>
   <si>
@@ -123,6 +120,21 @@
   </si>
   <si>
     <t>light blue: test targets</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in BoardInitTests) *Some of the white doors were highlighted a different color for current tests</t>
+  </si>
+  <si>
+    <t>*Dark blue cells are doors</t>
+  </si>
+  <si>
+    <t>*Yellow cells are walkways</t>
+  </si>
+  <si>
+    <t>*Grey cells are rooms</t>
+  </si>
+  <si>
+    <t>*Red cells are closets</t>
   </si>
 </sst>
 </file>
@@ -515,16 +527,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -587,7 +599,7 @@
       <c r="U1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -735,7 +747,7 @@
       <c r="S3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="U3" s="2" t="s">
@@ -794,7 +806,7 @@
       <c r="M4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -975,7 +987,7 @@
       <c r="V6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="X6" s="2" t="s">
@@ -1010,7 +1022,7 @@
       <c r="H7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1028,7 +1040,7 @@
       <c r="N7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -1105,10 +1117,10 @@
       <c r="N8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="7" t="s">
+      <c r="O8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Q8" s="2" t="s">
@@ -1194,7 +1206,7 @@
       <c r="R9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="S9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="T9" s="2" t="s">
@@ -1425,7 +1437,7 @@
       <c r="R12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S12" s="10" t="s">
+      <c r="S12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -1573,7 +1585,7 @@
       <c r="P14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -1688,7 +1700,7 @@
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1881,7 +1893,7 @@
       <c r="P18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="Q18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -1922,7 +1934,7 @@
       <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -1967,10 +1979,10 @@
       <c r="S19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="U19" s="4" t="s">
+      <c r="T19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U19" s="7" t="s">
         <v>19</v>
       </c>
       <c r="V19" s="1" t="s">
@@ -1979,7 +1991,7 @@
       <c r="W19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X19" s="2" t="s">
+      <c r="X19" s="10" t="s">
         <v>24</v>
       </c>
       <c r="Y19">
@@ -2044,7 +2056,7 @@
       <c r="S20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="T20" s="10" t="s">
         <v>24</v>
       </c>
       <c r="U20" s="1" t="s">
@@ -2150,10 +2162,10 @@
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -2183,7 +2195,7 @@
       <c r="N22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="10" t="s">
+      <c r="O22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -2195,7 +2207,7 @@
       <c r="R22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="T22" s="2" t="s">
@@ -2207,7 +2219,7 @@
       <c r="V22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="W22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="X22" s="2" t="s">
@@ -2292,38 +2304,58 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added excel file with layout
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddierogers/Documents/Mines Spring 2017/CSCI306/ClueGameMRFS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felig\workspace\ClueGameMRFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26320" windowHeight="12260"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="26318" windowHeight="12263"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -242,6 +242,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,13 +532,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +702,7 @@
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -766,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,8 +1000,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1074,8 +1077,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1151,7 +1154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1298,14 +1301,14 @@
       <c r="W10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="10" t="s">
         <v>24</v>
       </c>
       <c r="Y10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1321,7 +1324,7 @@
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -1382,7 +1385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1991,14 +1994,14 @@
       <c r="W19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X19" s="10" t="s">
+      <c r="X19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Y19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -2165,10 +2168,10 @@
       <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2229,131 +2232,131 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A23" s="11">
         <v>0</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="11">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="11">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="11">
         <v>3</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="11">
         <v>4</v>
       </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="11">
+        <v>5</v>
+      </c>
+      <c r="G23" s="11">
         <v>6</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="11">
         <v>7</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="11">
         <v>8</v>
       </c>
-      <c r="J23">
-        <v>9</v>
-      </c>
-      <c r="K23">
+      <c r="J23" s="11">
+        <v>9</v>
+      </c>
+      <c r="K23" s="11">
         <v>10</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="11">
         <v>11</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="11">
         <v>12</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="11">
         <v>13</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="11">
         <v>14</v>
       </c>
-      <c r="P23">
-        <v>15</v>
-      </c>
-      <c r="Q23">
+      <c r="P23" s="11">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="11">
         <v>16</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="11">
         <v>17</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="11">
         <v>18</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="11">
         <v>19</v>
       </c>
-      <c r="U23">
-        <v>20</v>
-      </c>
-      <c r="V23">
+      <c r="U23" s="11">
+        <v>20</v>
+      </c>
+      <c r="V23" s="11">
         <v>21</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="11">
         <v>22</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="11">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>

</xml_diff>